<commit_message>
sanofi Turkey template update
</commit_message>
<xml_diff>
--- a/Projects/SANOFITR/Data/Template.xlsx
+++ b/Projects/SANOFITR/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -1083,7 +1083,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="61">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1168,20 +1168,16 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1214,18 +1210,6 @@
     </xf>
     <xf numFmtId="164" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1424,20 +1408,20 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1174089068826"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.663967611336"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.8097165991903"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.0607287449393"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.4048582995951"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.0526315789474"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.2995951417004"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7287449392713"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1821862348178"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.4251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7732793522267"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3036437246964"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.9068825910931"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1694,21 +1678,21 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="27.5425101214575"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="47.2550607287449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="24.1174089068826"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="19.587044534413"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="14.8097165991903"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="19.587044534413"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="17.8744939271255"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="14" width="17.8744939271255"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="15" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="28.1578947368421"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="48.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="24.7287449392713"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="20.0728744939271"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="15.0526315789474"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="20.0728744939271"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="18.2388663967611"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="14" width="18.2388663967611"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="15" width="9.54655870445344"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1762,16 +1746,16 @@
       <c r="D3" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="25" t="n">
+      <c r="F3" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="24" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1788,16 +1772,16 @@
       <c r="D4" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="25" t="n">
+      <c r="F4" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="24" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1814,16 +1798,16 @@
       <c r="D5" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="25" t="n">
+      <c r="F5" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="24" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1840,16 +1824,16 @@
       <c r="D6" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="25" t="n">
+      <c r="F6" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1866,16 +1850,16 @@
       <c r="D7" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="25" t="n">
+      <c r="F7" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="24" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1892,16 +1876,16 @@
       <c r="D8" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="25" t="n">
+      <c r="F8" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="24" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1921,13 +1905,13 @@
       <c r="E9" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="25" t="n">
+      <c r="F9" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="24" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1947,13 +1931,13 @@
       <c r="E10" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="25" t="n">
+      <c r="F10" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="24" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1973,13 +1957,13 @@
       <c r="E11" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="25" t="n">
+      <c r="F11" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="24" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2005,290 +1989,290 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="27.5425101214575"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="26" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="34.1578947368421"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="26" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="26" width="18.7327935222672"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="14" width="18.1174089068826"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="15" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="28.1578947368421"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="25" width="23.6315789473684"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="25" width="34.8906882591093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="25" width="23.6315789473684"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="25" width="19.2186234817814"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="14" width="18.4898785425101"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="15" width="9.54655870445344"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="28" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="29" t="s">
+      <c r="A2" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="30" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="35" t="n">
+      <c r="E3" s="22" t="n">
         <v>8699693150011</v>
       </c>
-      <c r="F3" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="36" t="n">
+      <c r="F3" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="32" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="39" t="n">
+      <c r="E4" s="35" t="n">
         <v>8699693150080</v>
       </c>
-      <c r="F4" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="36" t="n">
+      <c r="F4" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="32" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="39" t="n">
+      <c r="E5" s="35" t="n">
         <v>8699693150172</v>
       </c>
-      <c r="F5" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="36" t="n">
+      <c r="F5" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="32" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="39" t="n">
+      <c r="E6" s="35" t="n">
         <v>8699693150189</v>
       </c>
-      <c r="F6" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="36" t="n">
+      <c r="F6" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="32" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="33" t="s">
         <v>45</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="39" t="n">
+      <c r="E7" s="35" t="n">
         <v>8699809706620</v>
       </c>
-      <c r="F7" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="36" t="n">
+      <c r="F7" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="32" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="33" t="s">
         <v>45</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="39" t="n">
+      <c r="E8" s="35" t="n">
         <v>8699809779181</v>
       </c>
-      <c r="F8" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="36" t="n">
+      <c r="F8" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="32" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="39" t="n">
+      <c r="E9" s="35" t="n">
         <v>8699809098558</v>
       </c>
-      <c r="F9" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="36" t="n">
+      <c r="F9" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="32" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="39" t="n">
+      <c r="E10" s="35" t="n">
         <v>8699809098770</v>
       </c>
-      <c r="F10" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="36" t="n">
+      <c r="F10" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="32" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="39" t="n">
+      <c r="E11" s="35" t="n">
         <v>8699809575202</v>
       </c>
-      <c r="F11" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="36" t="n">
+      <c r="F11" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="32" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2314,56 +2298,56 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="40" width="22.5222672064777"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="41.0121457489879"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="40" width="22.5222672064777"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="40" width="17.8744939271255"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="40" width="15.919028340081"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="41" width="20.4453441295547"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="42" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="36" width="23.0161943319838"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="36" width="41.9919028340081"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="36" width="23.0161943319838"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="36" width="18.2388663967611"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="36" width="16.1619433198381"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="37" width="20.9392712550607"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="38" width="9.54655870445344"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="43"/>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="28" t="s">
+      <c r="A1" s="39"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="29" t="s">
+      <c r="A2" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="30" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2389,271 +2373,271 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="31.2226720647773"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="45" width="35.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="26" width="24.1174089068826"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="45" width="28.7732793522267"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="45" width="20.8097165991903"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="20.3238866396761"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="26" width="19.587044534413"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="46" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="47" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="31.9514170040486"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="41" width="36.3643724696356"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="24.7287449392713"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="41" width="29.3805668016194"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="41" width="21.1821862348178"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="25" width="20.8097165991903"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="25" width="20.0728744939271"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="42" width="14.0769230769231"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="43" width="9.54655870445344"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="48"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="28" t="s">
+      <c r="A1" s="44"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="49" t="s">
+      <c r="A2" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="30" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="36" t="n">
+      <c r="F3" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="32" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="47" t="s">
         <v>45</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="36" t="n">
+      <c r="F4" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="32" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="36" t="n">
+      <c r="F5" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="32" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="51" t="s">
+      <c r="E6" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="36" t="n">
+      <c r="F6" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="32" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="51" t="s">
+      <c r="D7" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="36" t="n">
+      <c r="F7" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="32" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="51" t="s">
+      <c r="D8" s="47" t="s">
         <v>45</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="36" t="n">
+      <c r="F8" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="32" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="47" t="s">
         <v>45</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="36" t="n">
+      <c r="F9" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="32" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="53" t="s">
+      <c r="D10" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="51" t="s">
+      <c r="E10" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="36" t="n">
+      <c r="F10" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="32" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="54"/>
+      <c r="C11" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2677,291 +2661,291 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="55" width="34.1578947368421"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="55" width="47.2550607287449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="55" width="20.6882591093117"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="55" width="19.2186234817814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="55" width="17.8744939271255"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="55" width="19.587044534413"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="56" width="17.6234817813765"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="57" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="51" width="34.8906882591093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="51" width="48.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="51" width="21.1821862348178"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="51" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="51" width="18.2388663967611"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="51" width="20.0728744939271"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="52" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="53" width="9.54655870445344"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="58"/>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="28" t="s">
+      <c r="A1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="49" t="s">
+      <c r="A2" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="30" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="61" t="n">
+      <c r="C3" s="57" t="n">
         <v>8699693150011</v>
       </c>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="62" t="s">
+      <c r="E3" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="63" t="n">
+      <c r="F3" s="59" t="n">
         <v>6</v>
       </c>
-      <c r="G3" s="63" t="n">
+      <c r="G3" s="59" t="n">
         <v>3</v>
       </c>
-      <c r="H3" s="63" t="n">
+      <c r="H3" s="59" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="61" t="n">
+      <c r="C4" s="57" t="n">
         <v>8699693150080</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="62" t="s">
+      <c r="E4" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="63" t="n">
+      <c r="F4" s="59" t="n">
         <v>4</v>
       </c>
-      <c r="G4" s="63" t="n">
+      <c r="G4" s="59" t="n">
         <v>2</v>
       </c>
-      <c r="H4" s="63" t="n">
+      <c r="H4" s="59" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="64" t="n">
+      <c r="C5" s="60" t="n">
         <v>8699693150172</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="63" t="n">
+      <c r="F5" s="59" t="n">
         <v>2</v>
       </c>
-      <c r="G5" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="63" t="n">
+      <c r="G5" s="59" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="59" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="64" t="n">
+      <c r="C6" s="60" t="n">
         <v>8699693150189</v>
       </c>
-      <c r="D6" s="55" t="s">
+      <c r="D6" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="55" t="s">
+      <c r="E6" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="63" t="n">
+      <c r="F6" s="59" t="n">
         <v>2</v>
       </c>
-      <c r="G6" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="63" t="n">
+      <c r="G6" s="59" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="59" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="64" t="n">
+      <c r="C7" s="60" t="n">
         <v>8699809706620</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="51" t="s">
         <v>45</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="63" t="n">
+      <c r="F7" s="59" t="n">
         <v>2</v>
       </c>
-      <c r="G7" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="63" t="n">
+      <c r="G7" s="59" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="59" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="64" t="n">
+      <c r="C8" s="60" t="n">
         <v>8699809779181</v>
       </c>
-      <c r="D8" s="55" t="s">
+      <c r="D8" s="51" t="s">
         <v>45</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="63" t="n">
+      <c r="F8" s="59" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="63" t="n">
+      <c r="G8" s="59" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="59" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="64" t="n">
+      <c r="C9" s="60" t="n">
         <v>8699809098558</v>
       </c>
-      <c r="D9" s="55" t="s">
+      <c r="D9" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="55" t="s">
+      <c r="E9" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="63" t="n">
-        <v>1</v>
+      <c r="F9" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="59" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="64" t="n">
+      <c r="C10" s="60" t="n">
         <v>8699809098770</v>
       </c>
-      <c r="D10" s="55" t="s">
+      <c r="D10" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="55" t="s">
+      <c r="E10" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="63" t="n">
-        <v>1</v>
+      <c r="F10" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="59" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="64" t="n">
+      <c r="C11" s="60" t="n">
         <v>8699809575202</v>
       </c>
-      <c r="D11" s="55" t="s">
+      <c r="D11" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="55" t="s">
+      <c r="E11" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="63" t="n">
+      <c r="F11" s="59" t="n">
         <v>4</v>
       </c>
-      <c r="G11" s="63" t="n">
+      <c r="G11" s="59" t="n">
         <v>3</v>
       </c>
-      <c r="H11" s="63" t="n">
+      <c r="H11" s="59" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>